<commit_message>
update on multivariate analysis
</commit_message>
<xml_diff>
--- a/output/Death predictors/variable-importance.xlsx
+++ b/output/Death predictors/variable-importance.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -381,7 +381,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>0.08887551312358243</v>
+        <v>0.112391095218535</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -394,10 +394,10 @@
         </is>
       </c>
       <c r="B3">
-        <v>0.05326789250908869</v>
+        <v>0.08315687563982373</v>
       </c>
       <c r="C3">
-        <v>0.5993539799316723</v>
+        <v>0.7398884713965301</v>
       </c>
     </row>
     <row r="4">
@@ -407,10 +407,10 @@
         </is>
       </c>
       <c r="B4">
-        <v>0.0495376549476533</v>
+        <v>0.06844147957084062</v>
       </c>
       <c r="C4">
-        <v>0.5573824916067783</v>
+        <v>0.608958204720418</v>
       </c>
     </row>
     <row r="5">
@@ -420,23 +420,23 @@
         </is>
       </c>
       <c r="B5">
-        <v>0.03801261787405163</v>
+        <v>0.04261553014211164</v>
       </c>
       <c r="C5">
-        <v>0.4277063111995162</v>
+        <v>0.3791717667600741</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>ngs_result</t>
+          <t>scd8_f</t>
         </is>
       </c>
       <c r="B6">
-        <v>0.02404947995858529</v>
+        <v>0.04208040812602754</v>
       </c>
       <c r="C6">
-        <v>0.2705973683116092</v>
+        <v>0.3744105175254831</v>
       </c>
     </row>
     <row r="7">
@@ -446,10 +446,10 @@
         </is>
       </c>
       <c r="B7">
-        <v>0.020234642374115</v>
+        <v>0.03688598190165084</v>
       </c>
       <c r="C7">
-        <v>0.2276739864891525</v>
+        <v>0.3281930995505397</v>
       </c>
     </row>
     <row r="8">
@@ -459,257 +459,36 @@
         </is>
       </c>
       <c r="B8">
-        <v>0.01922868417919522</v>
+        <v>0.03478923955267799</v>
       </c>
       <c r="C8">
-        <v>0.2163552535832621</v>
+        <v>0.3095373302042591</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>neuropathy_sensory_min</t>
+          <t>tils3_class</t>
         </is>
       </c>
       <c r="B9">
-        <v>0.01543592035213995</v>
+        <v>0.01269128618488885</v>
       </c>
       <c r="C9">
-        <v>0.1736802389053566</v>
+        <v>0.1129207448349152</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>bmi</t>
+          <t>radio</t>
         </is>
       </c>
       <c r="B10">
-        <v>0.01402037677106177</v>
+        <v>0.002325011922407512</v>
       </c>
       <c r="C10">
-        <v>0.1577529769258972</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>total_cd8_f</t>
-        </is>
-      </c>
-      <c r="B11">
-        <v>0.01357679211197718</v>
-      </c>
-      <c r="C11">
-        <v>0.152761898466887</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>ki67_percent</t>
-        </is>
-      </c>
-      <c r="B12">
-        <v>0.01166942249766233</v>
-      </c>
-      <c r="C12">
-        <v>0.1313007608905263</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>histo_grade</t>
-        </is>
-      </c>
-      <c r="B13">
-        <v>0.011069027883342</v>
-      </c>
-      <c r="C13">
-        <v>0.124545304936247</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>tils3_class</t>
-        </is>
-      </c>
-      <c r="B14">
-        <v>0.01097944152881084</v>
-      </c>
-      <c r="C14">
-        <v>0.1235373067668684</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>cardiac_min</t>
-        </is>
-      </c>
-      <c r="B15">
-        <v>0.01028418450021402</v>
-      </c>
-      <c r="C15">
-        <v>0.1157144880380465</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>scd8_f</t>
-        </is>
-      </c>
-      <c r="B16">
-        <v>0.009619949172946068</v>
-      </c>
-      <c r="C16">
-        <v>0.1082407159727946</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>radio</t>
-        </is>
-      </c>
-      <c r="B17">
-        <v>0.008586660547153124</v>
-      </c>
-      <c r="C17">
-        <v>0.09661446944574344</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>prev_other_canc</t>
-        </is>
-      </c>
-      <c r="B18">
-        <v>0.008390581876938809</v>
-      </c>
-      <c r="C18">
-        <v>0.09440825242011945</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>location</t>
-        </is>
-      </c>
-      <c r="B19">
-        <v>0.0079204686338972</v>
-      </c>
-      <c r="C19">
-        <v>0.08911868247538214</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>cardiac_max</t>
-        </is>
-      </c>
-      <c r="B20">
-        <v>0.005979272323036229</v>
-      </c>
-      <c r="C20">
-        <v>0.06727693729004953</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>icd8_f</t>
-        </is>
-      </c>
-      <c r="B21">
-        <v>0.005978328410044225</v>
-      </c>
-      <c r="C21">
-        <v>0.06726631667072673</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>family_other_canc</t>
-        </is>
-      </c>
-      <c r="B22">
-        <v>0.00318861217379643</v>
-      </c>
-      <c r="C22">
-        <v>0.03587728567443125</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>neuropathy_motor_min</t>
-        </is>
-      </c>
-      <c r="B23">
-        <v>0.003012181732962909</v>
-      </c>
-      <c r="C23">
-        <v>0.03389214449625101</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>breast_surg_present</t>
-        </is>
-      </c>
-      <c r="B24">
-        <v>0.002369166268742653</v>
-      </c>
-      <c r="C24">
-        <v>0.02665713181816796</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>m_dist_metastasis</t>
-        </is>
-      </c>
-      <c r="B25">
-        <v>0.00204812904679802</v>
-      </c>
-      <c r="C25">
-        <v>0.0230449195151208</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>ps</t>
-        </is>
-      </c>
-      <c r="B26">
-        <v>0.001111056303606472</v>
-      </c>
-      <c r="C26">
-        <v>0.01250126457285862</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>histology_class</t>
-        </is>
-      </c>
-      <c r="B27">
-        <v>-0.001330258805382698</v>
-      </c>
-      <c r="C27">
-        <v>-0.01496766385509311</v>
+        <v>0.02068679834364744</v>
       </c>
     </row>
   </sheetData>

</xml_diff>